<commit_message>
added explanations in mapping
</commit_message>
<xml_diff>
--- a/Mappings/Wound - STU3.xlsx
+++ b/Mappings/Wound - STU3.xlsx
@@ -21,12 +21,12 @@
     <sheet name="WoundTypeCodelist" sheetId="12" r:id="rId12"/>
     <sheet name="Terms of Use" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="292">
   <si>
     <t>Subject</t>
   </si>
@@ -873,15 +873,6 @@
     <t>.code</t>
   </si>
   <si>
-    <t>.component.woundTissue.oncoUlcerList (codeableConcept)</t>
-  </si>
-  <si>
-    <t>.component.woundTissue.WCSCodeList (codeableConcept)</t>
-  </si>
-  <si>
-    <t>.component.woundInfection (codeableConcept)</t>
-  </si>
-  <si>
     <t>.component.woundMoistureCodelist (codeableConcept)</t>
   </si>
   <si>
@@ -907,13 +898,52 @@
 (extension, reference to BodySite Qualifier)</t>
   </si>
   <si>
-    <t>.drain (extension on extension-medicaldevice)</t>
-  </si>
-  <si>
     <t>.woundimage (extension, binary)</t>
   </si>
   <si>
     <t>.comment</t>
+  </si>
+  <si>
+    <t>.component.woundTissue.oncoUlcerList (slice, codeableConcept)</t>
+  </si>
+  <si>
+    <t>.component.woundTissue.WCSCodeList (slice, codeableConcept)</t>
+  </si>
+  <si>
+    <t>Not in effective[x], because effective[x] is for the datetime of the observation</t>
+  </si>
+  <si>
+    <t>Valueset</t>
+  </si>
+  <si>
+    <t>Equivalence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use code to define the observation. In .category we will use a more general snomed code to comprehend all types of wound, the hcim pressure ulcer and burnwound will have the same .category
+</t>
+  </si>
+  <si>
+    <t>HCIM
+Valueset is not fully compatible with .code..
+This is because in the valueset "Other" can be chosen, and in Code, "Other" isn't very pretty. If some ever searches all instances with code "other" then instances with this profile will pop up.. This isn't useful to anybody.</t>
+  </si>
+  <si>
+    <t>.component.woundInfection (codeableBoolean)</t>
+  </si>
+  <si>
+    <t>.component.woundEdge (codeableConcept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.woundDrain.valueReference.device.type, where
+• .woundDrain.valueReference.device (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct-WoundDrain)
+--&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDeviceProduct)
+</t>
+  </si>
+  <si>
+    <t>.woundDrain, where:
+• .woundDrain (extension http://nictiz.nl/fhir/StructureDefinition/extension-medicaldevice)
+• .woundDrain.valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice-WoundDrain)
+--&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1099,9 +1129,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1110,6 +1137,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1664,15 +1700,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
@@ -1804,15 +1840,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
@@ -1898,7 +1934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1910,15 +1948,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
@@ -2144,10 +2182,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
@@ -2357,10 +2395,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R20"/>
+  <dimension ref="B2:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2371,15 +2409,16 @@
     <col min="9" max="10" width="5" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="75" customWidth="1"/>
+    <col min="13" max="13" width="37.85546875" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="34.5703125" customWidth="1"/>
-    <col min="17" max="17" width="30" customWidth="1"/>
-    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="16" max="16" width="80" customWidth="1"/>
+    <col min="17" max="18" width="34.5703125" customWidth="1"/>
+    <col min="19" max="19" width="30" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18">
+    <row r="2" spans="2:20">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
@@ -2415,14 +2454,20 @@
       <c r="P2" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="25.5">
+    <row r="3" spans="2:20" ht="25.5">
       <c r="B3" s="8" t="s">
         <v>70</v>
       </c>
@@ -2447,13 +2492,15 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="2:18">
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="2:20" ht="127.5">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>75</v>
@@ -2484,13 +2531,19 @@
       <c r="O4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="2:18" ht="25.5">
+      <c r="Q4" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="2:20">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>83</v>
@@ -2499,58 +2552,66 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="20"/>
       <c r="O5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="P5" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="16"/>
-    </row>
-    <row r="6" spans="2:18" ht="25.5">
+      <c r="P5" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="20"/>
+    </row>
+    <row r="6" spans="2:20" ht="25.5">
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
       <c r="O6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="P6" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="16"/>
-    </row>
-    <row r="7" spans="2:18" ht="38.25">
+      <c r="P6" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="20"/>
+    </row>
+    <row r="7" spans="2:20" ht="38.25">
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
         <v>90</v>
@@ -2581,13 +2642,15 @@
         <v>95</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="2:18" ht="38.25">
+      <c r="P7" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="2:20" ht="38.25">
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
         <v>96</v>
@@ -2620,13 +2683,17 @@
       <c r="O8" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="P8" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="2:18" ht="38.25">
+      <c r="P8" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="2:20" ht="38.25">
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
         <v>102</v>
@@ -2659,13 +2726,17 @@
       <c r="O9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P9" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="2:18" ht="38.25">
+      <c r="P9" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="2:20" ht="38.25">
       <c r="B10" s="11"/>
       <c r="C10" s="12" t="s">
         <v>108</v>
@@ -2692,17 +2763,19 @@
       <c r="M10" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="17" t="s">
         <v>113</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="2:18" ht="38.25">
+      <c r="P10" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" spans="2:20" ht="38.25">
       <c r="B11" s="11"/>
       <c r="C11" s="12" t="s">
         <v>114</v>
@@ -2733,13 +2806,15 @@
         <v>118</v>
       </c>
       <c r="O11" s="2"/>
-      <c r="P11" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="2:18" ht="38.25">
+      <c r="P11" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="2:20" ht="38.25">
       <c r="B12" s="11"/>
       <c r="C12" s="12" t="s">
         <v>119</v>
@@ -2770,13 +2845,15 @@
         <v>123</v>
       </c>
       <c r="O12" s="2"/>
-      <c r="P12" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="2:18" ht="25.5">
+      <c r="P12" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="2"/>
+    </row>
+    <row r="13" spans="2:20" ht="25.5">
       <c r="B13" s="11"/>
       <c r="C13" s="12" t="s">
         <v>124</v>
@@ -2809,13 +2886,17 @@
       <c r="O13" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="P13" s="19" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="2:18" ht="38.25">
+      <c r="P13" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q13" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R13" s="18"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="2"/>
+    </row>
+    <row r="14" spans="2:20" ht="38.25">
       <c r="B14" s="11"/>
       <c r="C14" s="12" t="s">
         <v>130</v>
@@ -2848,13 +2929,17 @@
       <c r="O14" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="P14" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="2:18">
+      <c r="P14" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="18"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="2"/>
+    </row>
+    <row r="15" spans="2:20" ht="38.25">
       <c r="B15" s="11"/>
       <c r="C15" s="12" t="s">
         <v>136</v>
@@ -2883,13 +2968,17 @@
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="19" t="s">
-        <v>278</v>
+      <c r="P15" s="18" t="s">
+        <v>275</v>
       </c>
       <c r="Q15" s="18"/>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="2:18" ht="25.5">
+      <c r="R15" s="18"/>
+      <c r="S15" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="T15" s="2"/>
+    </row>
+    <row r="16" spans="2:20" ht="25.5">
       <c r="B16" s="11"/>
       <c r="C16" s="12" t="s">
         <v>141</v>
@@ -2918,13 +3007,15 @@
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="2:18" ht="38.25">
+      <c r="P16" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="2"/>
+    </row>
+    <row r="17" spans="2:20" ht="63.75">
       <c r="B17" s="11"/>
       <c r="C17" s="12" t="s">
         <v>145</v>
@@ -2955,13 +3046,15 @@
       <c r="O17" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="P17" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="2:18">
+      <c r="P17" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="2"/>
+    </row>
+    <row r="18" spans="2:20" ht="63.75">
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
@@ -2990,11 +3083,17 @@
       <c r="O18" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="2:18">
+      <c r="P18" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q18" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="2"/>
+    </row>
+    <row r="19" spans="2:20">
       <c r="B19" s="11"/>
       <c r="C19" s="12" t="s">
         <v>157</v>
@@ -3023,13 +3122,15 @@
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="2:18" ht="25.5">
+      <c r="P19" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="2"/>
+    </row>
+    <row r="20" spans="2:20" ht="25.5">
       <c r="B20" s="11"/>
       <c r="C20" s="12" t="s">
         <v>163</v>
@@ -3060,17 +3161,19 @@
         <v>168</v>
       </c>
       <c r="O20" s="2"/>
-      <c r="P20" s="18" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="2"/>
+      <c r="P20" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="M5:M6"/>
     <mergeCell ref="N5:N6"/>
-    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="T5:T6"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
@@ -3110,11 +3213,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3166,11 +3269,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:5">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3224,15 +3327,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
@@ -3364,15 +3467,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">
@@ -3470,15 +3573,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" spans="3:7">
       <c r="C4" s="14" t="s">

</xml_diff>

<commit_message>
added some more explaining in tab Research
</commit_message>
<xml_diff>
--- a/Mappings/Wound - STU3.xlsx
+++ b/Mappings/Wound - STU3.xlsx
@@ -10,23 +10,24 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
-    <sheet name="WoundAnatomicalLocationCodelist" sheetId="5" r:id="rId5"/>
-    <sheet name="WoundDrainTypeCodelist" sheetId="6" r:id="rId6"/>
-    <sheet name="WoundEdgeCodelist" sheetId="7" r:id="rId7"/>
-    <sheet name="WoundLateralityCodelist" sheetId="8" r:id="rId8"/>
-    <sheet name="WoundMoistureCodelist" sheetId="9" r:id="rId9"/>
-    <sheet name="WoundTissueOncoUlcerCodelist" sheetId="10" r:id="rId10"/>
-    <sheet name="WoundTissueWCSCodelist" sheetId="11" r:id="rId11"/>
-    <sheet name="WoundTypeCodelist" sheetId="12" r:id="rId12"/>
-    <sheet name="Terms of Use" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" r:id="rId5"/>
+    <sheet name="WoundAnatomicalLocationCodelist" sheetId="5" r:id="rId6"/>
+    <sheet name="WoundDrainTypeCodelist" sheetId="6" r:id="rId7"/>
+    <sheet name="WoundEdgeCodelist" sheetId="7" r:id="rId8"/>
+    <sheet name="WoundLateralityCodelist" sheetId="8" r:id="rId9"/>
+    <sheet name="WoundMoistureCodelist" sheetId="9" r:id="rId10"/>
+    <sheet name="WoundTissueOncoUlcerCodelist" sheetId="10" r:id="rId11"/>
+    <sheet name="WoundTissueWCSCodelist" sheetId="11" r:id="rId12"/>
+    <sheet name="WoundTypeCodelist" sheetId="12" r:id="rId13"/>
+    <sheet name="Terms of Use" sheetId="13" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="311">
   <si>
     <t>Subject</t>
   </si>
@@ -945,12 +946,70 @@
 • .woundDrain.valueReference (profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice-WoundDrain)
 --&gt; (derived from profile http://nictiz.nl/fhir/StructureDefinition/zib-MedicalDevice)</t>
   </si>
+  <si>
+    <t>Checkbox searched for existing profiles / implementation on:</t>
+  </si>
+  <si>
+    <t>Checkbox!</t>
+  </si>
+  <si>
+    <t>Searchwords</t>
+  </si>
+  <si>
+    <t>Found results:</t>
+  </si>
+  <si>
+    <t>Relevance:</t>
+  </si>
+  <si>
+    <t>HL7 FHIR Specification</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles - latest version latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry - latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR implementation guides (e.g. Argonaut)</t>
+  </si>
+  <si>
+    <t>Simplifier.net</t>
+  </si>
+  <si>
+    <t>Zulip (chat.fhir.org)</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google </t>
+  </si>
+  <si>
+    <t>wound</t>
+  </si>
+  <si>
+    <t>wound hl7 fhir</t>
+  </si>
+  <si>
+    <t>https://cimi.hl7.org/submissions/september_2018/skinwoundig/simplcimi/site/index.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIMI has a completely different approach to profiling as we do. CIMI sees every measurement as a seperate Observation. 
+For us, this is not useable. We are combining different measurements in one profile. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -991,6 +1050,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1079,10 +1150,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1147,8 +1219,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1159,6 +1241,126 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1268,6 +1470,1241 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14337" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14337"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14338" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14338"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14339" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14339"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14340" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14340"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14341" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14341"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14342" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14342"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14343" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14343"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14344" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14344"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14345" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14345"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14346" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14346"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14347" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14347"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14348" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14348"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14349" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14349"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14350" name="Check Box 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14350"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14351" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14351"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14352" name="Check Box 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14352"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14353" name="Check Box 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14353"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14354" name="Check Box 18" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14354"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14355" name="Check Box 19" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14355"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14356" name="Check Box 20" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14356"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14357" name="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14357"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14358" name="Check Box 22" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14358"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14359" name="Check Box 23" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14359"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>180975</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14360" name="Check Box 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14360"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14361" name="Check Box 25" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14361"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14362" name="Check Box 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14362"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14363" name="Check Box 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14363"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14364" name="Check Box 28" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14364"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14365" name="Check Box 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14365"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>47625</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="14366" name="Check Box 30" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s14366"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1686,6 +3123,112 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="28" customWidth="1"/>
+    <col min="7" max="7" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7">
+      <c r="C3" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="25.5">
+      <c r="C5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" ht="25.5">
+      <c r="C6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="25.5">
+      <c r="C7" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D5:D7" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1824,7 +3367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G7"/>
   <sheetViews>
@@ -1930,7 +3473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G12"/>
   <sheetViews>
@@ -2123,7 +3666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>
@@ -2394,10 +3937,791 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="75.5703125" customWidth="1"/>
+    <col min="5" max="5" width="71.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="O1" s="22"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="23" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="38.25">
+      <c r="A10" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="C10" t="s">
+        <v>308</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>310</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14337" r:id="rId4" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14338" r:id="rId5" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14339" r:id="rId6" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>1</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14340" r:id="rId7" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14341" r:id="rId8" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14342" r:id="rId9" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14343" r:id="rId10" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14344" r:id="rId11" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14345" r:id="rId12" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14346" r:id="rId13" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14347" r:id="rId14" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14348" r:id="rId15" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14349" r:id="rId16" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14350" r:id="rId17" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14351" r:id="rId18" name="Check Box 15">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14352" r:id="rId19" name="Check Box 16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14353" r:id="rId20" name="Check Box 17">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14354" r:id="rId21" name="Check Box 18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14355" r:id="rId22" name="Check Box 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14356" r:id="rId23" name="Check Box 20">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14357" r:id="rId24" name="Check Box 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14358" r:id="rId25" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14359" r:id="rId26" name="Check Box 23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14360" r:id="rId27" name="Check Box 24">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14361" r:id="rId28" name="Check Box 25">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14362" r:id="rId29" name="Check Box 26">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14363" r:id="rId30" name="Check Box 27">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14364" r:id="rId31" name="Check Box 28">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14365" r:id="rId32" name="Check Box 29">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="14366" r:id="rId33" name="Check Box 30">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
@@ -3199,7 +5523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E5"/>
   <sheetViews>
@@ -3255,7 +5579,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E5"/>
   <sheetViews>
@@ -3311,7 +5635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G9"/>
   <sheetViews>
@@ -3447,112 +5771,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="D5:D9" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="32" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
-      <c r="C4" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7">
-      <c r="C5" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:G3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="D5:D7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3574,11 +5792,11 @@
   <sheetData>
     <row r="3" spans="3:7">
       <c r="C3" s="19" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
@@ -3600,55 +5818,55 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="25.5">
+    <row r="5" spans="3:7">
       <c r="C5" s="2" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" ht="25.5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
       <c r="C6" s="2" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="25.5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7">
       <c r="C7" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: zib-wound and zib-pressureUlcer both finished. todo: examples
</commit_message>
<xml_diff>
--- a/Mappings/Wound - STU3.xlsx
+++ b/Mappings/Wound - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -989,9 +989,6 @@
     <t>Observation(woundObservable).component.woundDepth (quantity, ucum)</t>
   </si>
   <si>
-    <t>Media</t>
-  </si>
-  <si>
     <t>.note</t>
   </si>
   <si>
@@ -1003,6 +1000,9 @@
   </si>
   <si>
     <t>.dateOfLastDressingChange (extension, datetime)</t>
+  </si>
+  <si>
+    <t>Observation(woundObservable).woundPhoto (extension)</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1390,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1431,7 +1431,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1472,7 +1472,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3027,7 +3027,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -3510,7 +3512,7 @@
   <dimension ref="C3:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E3" sqref="E3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4755,8 +4757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4897,7 +4899,7 @@
       </c>
       <c r="R4" s="17"/>
       <c r="S4" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="T4" s="2"/>
     </row>
@@ -5327,7 +5329,7 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="25" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q15" s="18"/>
       <c r="R15" s="18"/>
@@ -5364,7 +5366,7 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
@@ -5479,7 +5481,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="17" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="Q19" s="17"/>
       <c r="R19" s="17"/>
@@ -5518,7 +5520,7 @@
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>

</xml_diff>

<commit_message>
wip: amended mapping zib-wound
</commit_message>
<xml_diff>
--- a/Mappings/Wound - STU3.xlsx
+++ b/Mappings/Wound - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="4"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1390,7 +1390,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1431,7 +1431,7 @@
         <xdr:cNvPr id="1026" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1472,7 +1472,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4757,8 +4757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="M13" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5617,7 +5617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>

</xml_diff>